<commit_message>
no fill toegepast in wervingsgebieden-gestructureerd.xlsx
</commit_message>
<xml_diff>
--- a/Data/wervingsgebieden-gestructureerd.xlsx
+++ b/Data/wervingsgebieden-gestructureerd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svdberg\Documents\GitHub\POC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DF74BE6C-69A2-408F-AA23-9C1C022C286F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{85729DEF-6716-42B4-B5D5-820A5728E700}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{223288CE-0AF3-4D53-A7C7-97AA89081585}"/>
   </bookViews>
@@ -325,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,12 +503,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -672,7 +666,7 @@
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -682,27 +676,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1061,7 +1041,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,13 +1222,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="8">
         <v>3840</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>3859</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1259,13 +1239,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="8">
         <v>3860</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>3899</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1276,13 +1256,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="8">
         <v>7300</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="9">
         <v>7399</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1293,13 +1273,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="8">
         <v>7700</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="9">
         <v>7739</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1310,13 +1290,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="8">
         <v>7740</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="9">
         <v>7799</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1327,13 +1307,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="8">
         <v>7800</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="9">
         <v>7899</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1344,13 +1324,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="8">
         <v>7900</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="9">
         <v>7939</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1361,13 +1341,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="8">
         <v>8200</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="9">
         <v>8249</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1378,16 +1358,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="8">
         <v>7400</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="9">
         <v>7439</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1395,149 +1375,149 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="8">
         <v>7440</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="9">
         <v>7469</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="8">
         <v>7470</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="9">
         <v>7499</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="8">
         <v>7600</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="9">
         <v>7669</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="8">
         <v>7670</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="9">
         <v>7699</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="8">
         <v>7800</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="9">
         <v>7899</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="8">
         <v>8400</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="9">
         <v>8439</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="8">
         <v>8440</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="9">
         <v>8499</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="8">
         <v>9400</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="9">
         <v>9499</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="8">
         <v>1300</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="9">
         <v>1379</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D28" t="s">
@@ -1548,16 +1528,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="8">
         <v>8200</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="9">
         <v>8249</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E29" t="s">
@@ -1565,291 +1545,291 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="8">
         <v>1000</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="9">
         <v>1119</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="8">
         <v>1120</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="9">
         <v>1159</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="A32" s="8">
         <v>1200</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="9">
         <v>1249</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+      <c r="A33" s="8">
         <v>1250</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="9">
         <v>1269</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="A34" s="8">
         <v>1270</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="9">
         <v>1299</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
+      <c r="A35" s="8">
         <v>1380</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="9">
         <v>1399</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
+      <c r="A36" s="8">
         <v>1400</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="9">
         <v>1419</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
+      <c r="A37" s="8">
         <v>1420</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="9">
         <v>1439</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
+      <c r="A38" s="8">
         <v>1440</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="9">
         <v>1499</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
+      <c r="A39" s="8">
         <v>1500</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="9">
         <v>1519</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
+      <c r="A40" s="8">
         <v>1520</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="9">
         <v>1599</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
+      <c r="A41" s="8">
         <v>3700</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="9">
         <v>3719</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
+      <c r="A42" s="8">
         <v>3720</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="9">
         <v>3739</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
+      <c r="A43" s="8">
         <v>3740</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="9">
         <v>3769</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
+      <c r="A44" s="8">
         <v>3800</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="9">
         <v>3839</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+      <c r="A45" s="8">
         <v>3840</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="9">
         <v>3859</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
+      <c r="A46" s="8">
         <v>3860</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="9">
         <v>3899</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>